<commit_message>
Add files for 01-Excel/3
</commit_message>
<xml_diff>
--- a/01-Lesson-Plans/01-Excel/3/Activities/02-Ins_BasicCharting/Solved/basic_charts.xlsx
+++ b/01-Lesson-Plans/01-Excel/3/Activities/02-Ins_BasicCharting/Solved/basic_charts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dcorless/Documents/coding-boot-camp/DataViz-Lesson-Plans/01-Lesson-Plans/01-Excel/3/Activities/02-Ins_BasicCharting/Solved/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e8512a5b4b9cbd9d/UCB/temp/UCB-VIRT-DATA-PT-08-2023-U-LOLC/01-Lesson-Plans/01-Excel/3/Activities/02-Ins_BasicCharting/Solved/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD8C936-385F-5A4E-A05B-D4CBA8A2CD2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{CFD8C936-385F-5A4E-A05B-D4CBA8A2CD2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1AD902D0-B990-4444-AC94-A9AAA84654B0}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="14620" windowHeight="14080" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Favorite Ice Cream Flavors" sheetId="1" r:id="rId1"/>
@@ -1343,6 +1343,358 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="106"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="6"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Favorite Ice Cream Flavors'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Number of Faves</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="narHorz">
+                <a:fgClr>
+                  <a:schemeClr val="accent4">
+                    <a:shade val="65000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="accent4">
+                    <a:shade val="65000"/>
+                    <a:lumMod val="20000"/>
+                    <a:lumOff val="80000"/>
+                  </a:schemeClr>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:innerShdw blurRad="114300">
+                  <a:schemeClr val="accent4">
+                    <a:shade val="65000"/>
+                  </a:schemeClr>
+                </a:innerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="narHorz">
+                <a:fgClr>
+                  <a:schemeClr val="accent4"/>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="20000"/>
+                    <a:lumOff val="80000"/>
+                  </a:schemeClr>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:innerShdw blurRad="114300">
+                  <a:schemeClr val="accent4"/>
+                </a:innerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="narHorz">
+                <a:fgClr>
+                  <a:schemeClr val="accent4">
+                    <a:tint val="65000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="accent4">
+                    <a:tint val="65000"/>
+                    <a:lumMod val="20000"/>
+                    <a:lumOff val="80000"/>
+                  </a:schemeClr>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:innerShdw blurRad="114300">
+                  <a:schemeClr val="accent4">
+                    <a:tint val="65000"/>
+                  </a:schemeClr>
+                </a:innerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="25000"/>
+                    <a:lumOff val="75000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="wedgeRectCallout">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Favorite Ice Cream Flavors'!$A$2:$A$11</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>('Favorite Ice Cream Flavors'!$A$3:$A$4,'Favorite Ice Cream Flavors'!$A$8)</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Chocolate</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Strawberry</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Butter Pecan</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Favorite Ice Cream Flavors'!$B$2:$B$11</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>('Favorite Ice Cream Flavors'!$B$3:$B$4,'Favorite Ice Cream Flavors'!$B$8)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>96</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:categoryFilterExceptions/>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0079-4D81-9CBC-437970822F34}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="0"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
       <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
@@ -2974,6 +3326,12 @@
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="17">
+  <a:schemeClr val="accent4"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4033,6 +4391,525 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="203">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narHorz">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narHorz">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" cap="all" spc="150" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4617,6 +5494,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>441325</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>688975</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88C53121-FF7B-EC2C-5146-DA3D29CC2AD9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4965,16 +5878,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="8" width="20.6640625" customWidth="1"/>
+    <col min="1" max="8" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -4987,7 +5900,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4999,7 +5912,7 @@
         <v>0.11166666666666666</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -5011,7 +5924,7 @@
         <v>8.8333333333333333E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -5023,7 +5936,7 @@
         <v>0.10666666666666667</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -5035,7 +5948,7 @@
         <v>0.15666666666666668</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -5047,7 +5960,7 @@
         <v>9.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -5059,7 +5972,7 @@
         <v>0.13166666666666665</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -5071,7 +5984,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -5083,7 +5996,7 @@
         <v>6.8333333333333329E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -5095,7 +6008,7 @@
         <v>5.6666666666666664E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -5107,12 +6020,12 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15">
         <f>SUM(B2:B11)</f>
         <v>600</v>
@@ -5129,17 +6042,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="8" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.6328125" customWidth="1"/>
+    <col min="2" max="8" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>14</v>
       </c>
@@ -5174,7 +6087,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -5212,7 +6125,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -5250,7 +6163,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -5288,7 +6201,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -5326,7 +6239,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -5364,7 +6277,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -5402,7 +6315,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -5440,7 +6353,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -5478,7 +6391,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -5516,7 +6429,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>

</xml_diff>